<commit_message>
rules storage, schedule_generate based on given rules(untested)
</commit_message>
<xml_diff>
--- a/freelancer_schedule_weighted_randomization.xlsx
+++ b/freelancer_schedule_weighted_randomization.xlsx
@@ -863,12 +863,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -905,12 +905,12 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -969,7 +969,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -979,7 +979,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1122,12 +1122,12 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1149,7 +1149,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1164,7 +1164,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1440,7 +1440,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
     </row>

</xml_diff>